<commit_message>
Estructura y comienzo. Tests fallando
</commit_message>
<xml_diff>
--- a/IntNovAction.Utils.ExcelImporter.Tests/SampleExcels/SampleExcel.xlsx
+++ b/IntNovAction.Utils.ExcelImporter.Tests/SampleExcels/SampleExcel.xlsx
@@ -3,12 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{659BB9E9-D618-4A51-B9E6-4AC0BCE410C7}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{476D1FEF-E6D9-47FB-99B4-1A0BBADFF923}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="TypesOK" sheetId="2" r:id="rId1"/>
+    <sheet name="TypesWithErrors" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="13">
   <si>
     <t>Item 1</t>
   </si>
@@ -34,9 +35,6 @@
     <t>Item 4</t>
   </si>
   <si>
-    <t>IntColumn</t>
-  </si>
-  <si>
     <t>String Column</t>
   </si>
   <si>
@@ -53,6 +51,15 @@
   </si>
   <si>
     <t>N</t>
+  </si>
+  <si>
+    <t>Int Column</t>
+  </si>
+  <si>
+    <t>Item 5</t>
+  </si>
+  <si>
+    <t>S</t>
   </si>
 </sst>
 </file>
@@ -370,11 +377,110 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD8FBFDA-237A-49E6-9F7D-0EE6B0BBA225}">
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1">
+        <v>36526</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1">
+        <v>36527</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1">
+        <v>36528</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1">
+        <v>36529</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="1">
+        <v>36530</v>
+      </c>
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -386,16 +492,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
-        <v>6</v>
-      </c>
       <c r="D1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -423,7 +529,7 @@
         <v>37253</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -445,12 +551,12 @@
         <v>43132</v>
       </c>
       <c r="D5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
Support for Decimal, Float, Date, String fields
</commit_message>
<xml_diff>
--- a/IntNovAction.Utils.ExcelImporter.Tests/SampleExcels/SampleExcel.xlsx
+++ b/IntNovAction.Utils.ExcelImporter.Tests/SampleExcels/SampleExcel.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{9A5D1713-C12D-41B9-8587-E7FA26A0829C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{E052224D-E2CF-4529-AA3C-C9069A162A58}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="19">
   <si>
     <t>Item 1</t>
   </si>
@@ -63,6 +63,21 @@
   </si>
   <si>
     <t>Nullable Int Column</t>
+  </si>
+  <si>
+    <t>Decimal Column</t>
+  </si>
+  <si>
+    <t>Nullable Decimal Column</t>
+  </si>
+  <si>
+    <t>Float Column</t>
+  </si>
+  <si>
+    <t>Nullable Float Column</t>
+  </si>
+  <si>
+    <t>Nullable Date Column</t>
   </si>
 </sst>
 </file>
@@ -390,111 +405,194 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD8FBFDA-237A-49E6-9F7D-0EE6B0BBA225}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
       <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" t="s">
         <v>13</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
+        <v>1.25</v>
+      </c>
+      <c r="C2">
+        <v>1.25</v>
+      </c>
+      <c r="D2">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2">
+        <v>1.25</v>
+      </c>
+      <c r="F2">
+        <v>1.25</v>
+      </c>
+      <c r="G2" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="1">
+      <c r="H2" s="1">
         <v>36526</v>
       </c>
-      <c r="E2">
+      <c r="I2" s="1">
+        <v>36526</v>
+      </c>
+      <c r="J2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" t="s">
+      <c r="B3">
+        <v>2.25</v>
+      </c>
+      <c r="C3">
+        <v>2.25</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="G3" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="1">
+      <c r="H3" s="1">
         <v>36527</v>
       </c>
-      <c r="E3" t="s">
+      <c r="I3" s="1"/>
+      <c r="J3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
+        <v>3.75</v>
+      </c>
+      <c r="C4">
+        <v>3.75</v>
+      </c>
+      <c r="D4">
         <v>3</v>
       </c>
-      <c r="C4" t="s">
+      <c r="E4">
+        <v>3.75</v>
+      </c>
+      <c r="F4">
+        <v>3.75</v>
+      </c>
+      <c r="G4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="1">
+      <c r="H4" s="1">
         <v>36528</v>
       </c>
-      <c r="E4">
+      <c r="I4" s="1">
+        <v>36528</v>
+      </c>
+      <c r="J4">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>5</v>
-      </c>
-      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>4.25</v>
+      </c>
+      <c r="C5">
+        <v>4.25</v>
+      </c>
+      <c r="G5" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="1">
+      <c r="H5" s="1">
         <v>36529</v>
       </c>
-      <c r="E5" t="s">
+      <c r="I5" s="1"/>
+      <c r="J5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6">
         <v>6</v>
       </c>
-      <c r="B6">
-        <v>6</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="E6">
+        <v>5</v>
+      </c>
+      <c r="F6">
+        <v>5</v>
+      </c>
+      <c r="G6" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="1">
+      <c r="H6" s="1">
         <v>36530</v>
       </c>
-      <c r="E6" t="s">
+      <c r="I6" s="1">
+        <v>36530</v>
+      </c>
+      <c r="J6" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Changes in the tests, error strategy
</commit_message>
<xml_diff>
--- a/IntNovAction.Utils.ExcelImporter.Tests/SampleExcels/SampleExcel.xlsx
+++ b/IntNovAction.Utils.ExcelImporter.Tests/SampleExcels/SampleExcel.xlsx
@@ -3,13 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{E052224D-E2CF-4529-AA3C-C9069A162A58}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{9BFBC4EA-55B1-499D-A201-56665D41E9C7}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="TypesOK" sheetId="2" r:id="rId1"/>
-    <sheet name="TypesWithErrors" sheetId="1" r:id="rId2"/>
+    <sheet name="Data OK" sheetId="2" r:id="rId1"/>
+    <sheet name="Data With Errors" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="20">
   <si>
     <t>Item 1</t>
   </si>
@@ -41,9 +41,6 @@
     <t>Date Column</t>
   </si>
   <si>
-    <t>aaaaa</t>
-  </si>
-  <si>
     <t>Bool column</t>
   </si>
   <si>
@@ -78,13 +75,19 @@
   </si>
   <si>
     <t>Nullable Date Column</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>a</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -94,6 +97,14 @@
     </font>
     <font>
       <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -121,10 +132,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -407,8 +419,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD8FBFDA-237A-49E6-9F7D-0EE6B0BBA225}">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -426,35 +438,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" t="s">
+      <c r="A1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="G1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" t="s">
-        <v>18</v>
-      </c>
-      <c r="J1" t="s">
-        <v>7</v>
+      <c r="J1" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -508,7 +520,7 @@
       </c>
       <c r="I3" s="1"/>
       <c r="J3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -561,7 +573,7 @@
       </c>
       <c r="I5" s="1"/>
       <c r="J5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -584,7 +596,7 @@
         <v>5</v>
       </c>
       <c r="G6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H6" s="1">
         <v>36530</v>
@@ -593,7 +605,7 @@
         <v>36530</v>
       </c>
       <c r="J6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -604,92 +616,188 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="1">
-        <v>36526</v>
+      <c r="B2">
+        <v>1.25</v>
+      </c>
+      <c r="C2">
+        <v>1.25</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="E2">
+        <v>1.25</v>
+      </c>
+      <c r="F2">
+        <v>1.25</v>
+      </c>
+      <c r="G2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" s="1">
+        <v>36526</v>
+      </c>
+      <c r="I2" s="1">
+        <v>36526</v>
+      </c>
+      <c r="J2">
         <v>1</v>
       </c>
-      <c r="C3" s="1">
-        <v>37253</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D3" s="2"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4">
+        <v>3.75</v>
+      </c>
+      <c r="C4">
+        <v>3.75</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>3.75</v>
+      </c>
+      <c r="F4">
+        <v>3.75</v>
+      </c>
+      <c r="G4" t="s">
         <v>2</v>
       </c>
-      <c r="D4">
+      <c r="H4" s="1">
+        <v>36528</v>
+      </c>
+      <c r="I4" s="1">
+        <v>36528</v>
+      </c>
+      <c r="J4">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>5</v>
-      </c>
-      <c r="C5" s="1">
-        <v>43132</v>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
       </c>
       <c r="D5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6">
         <v>6</v>
       </c>
-      <c r="B6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6">
-        <v>15000</v>
+      <c r="E6">
+        <v>5</v>
+      </c>
+      <c r="F6">
+        <v>5</v>
+      </c>
+      <c r="G6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="1">
+        <v>36530</v>
+      </c>
+      <c r="I6" s="1">
+        <v>36530</v>
+      </c>
+      <c r="J6" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Enable configuration for boolean strings, more complete readme
</commit_message>
<xml_diff>
--- a/IntNovAction.Utils.ExcelImporter.Tests/SampleExcels/SampleExcel.xlsx
+++ b/IntNovAction.Utils.ExcelImporter.Tests/SampleExcels/SampleExcel.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{9BFBC4EA-55B1-499D-A201-56665D41E9C7}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{BDA6F7FE-B4AC-42B2-A631-A4F4E02670B7}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data OK" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="23">
   <si>
     <t>Item 1</t>
   </si>
@@ -41,9 +41,6 @@
     <t>Date Column</t>
   </si>
   <si>
-    <t>Bool column</t>
-  </si>
-  <si>
     <t>Y</t>
   </si>
   <si>
@@ -81,6 +78,18 @@
   </si>
   <si>
     <t>a</t>
+  </si>
+  <si>
+    <t>Nullable Boolean column</t>
+  </si>
+  <si>
+    <t>Boolean column</t>
+  </si>
+  <si>
+    <t>SDDD</t>
+  </si>
+  <si>
+    <t>DDD</t>
   </si>
 </sst>
 </file>
@@ -417,10 +426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD8FBFDA-237A-49E6-9F7D-0EE6B0BBA225}">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:J6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -437,24 +446,24 @@
     <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>15</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>16</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>4</v>
@@ -463,13 +472,16 @@
         <v>5</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -500,8 +512,11 @@
       <c r="J2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -520,10 +535,10 @@
       </c>
       <c r="I3" s="1"/>
       <c r="J3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -554,8 +569,11 @@
       <c r="J4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -573,10 +591,10 @@
       </c>
       <c r="I5" s="1"/>
       <c r="J5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -596,7 +614,7 @@
         <v>5</v>
       </c>
       <c r="G6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H6" s="1">
         <v>36530</v>
@@ -605,7 +623,10 @@
         <v>36530</v>
       </c>
       <c r="J6" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="K6" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -616,10 +637,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -633,26 +654,27 @@
     <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>15</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>16</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>4</v>
@@ -661,13 +683,16 @@
         <v>5</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -698,13 +723,22 @@
       <c r="J2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D3" s="2"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -735,40 +769,46 @@
       <c r="J4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="K5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -788,7 +828,7 @@
         <v>5</v>
       </c>
       <c r="G6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H6" s="1">
         <v>36530</v>
@@ -797,7 +837,10 @@
         <v>36530</v>
       </c>
       <c r="J6" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="K6" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Can specify duplicated column strategy
</commit_message>
<xml_diff>
--- a/IntNovAction.Utils.ExcelImporter.Tests/SampleExcels/SampleExcel.xlsx
+++ b/IntNovAction.Utils.ExcelImporter.Tests/SampleExcels/SampleExcel.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{BDA6F7FE-B4AC-42B2-A631-A4F4E02670B7}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{525AD291-8C99-44A1-ADB7-A0376FF619C0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data OK" sheetId="2" r:id="rId1"/>
     <sheet name="Data With Errors" sheetId="1" r:id="rId2"/>
+    <sheet name="Duplicated Columns" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="23">
   <si>
     <t>Item 1</t>
   </si>
@@ -428,8 +429,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD8FBFDA-237A-49E6-9F7D-0EE6B0BBA225}">
   <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -847,4 +848,233 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A672CE3F-A506-4424-8FD9-AF8F875076FD}">
+  <dimension ref="A1:L6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1.25</v>
+      </c>
+      <c r="C2">
+        <v>1.25</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1.25</v>
+      </c>
+      <c r="F2">
+        <v>1.25</v>
+      </c>
+      <c r="G2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" s="1">
+        <v>36526</v>
+      </c>
+      <c r="I2" s="1">
+        <v>36526</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>2.25</v>
+      </c>
+      <c r="C3">
+        <v>2.25</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="G3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H3" s="1">
+        <v>36527</v>
+      </c>
+      <c r="I3" s="1"/>
+      <c r="J3" t="s">
+        <v>6</v>
+      </c>
+      <c r="L3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>3.75</v>
+      </c>
+      <c r="C4">
+        <v>3.75</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>3.75</v>
+      </c>
+      <c r="F4">
+        <v>3.75</v>
+      </c>
+      <c r="G4" t="s">
+        <v>2</v>
+      </c>
+      <c r="H4" s="1">
+        <v>36528</v>
+      </c>
+      <c r="I4" s="1">
+        <v>36528</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>4.25</v>
+      </c>
+      <c r="C5">
+        <v>4.25</v>
+      </c>
+      <c r="G5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H5" s="1">
+        <v>36529</v>
+      </c>
+      <c r="I5" s="1"/>
+      <c r="J5" t="s">
+        <v>7</v>
+      </c>
+      <c r="L5">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <v>6</v>
+      </c>
+      <c r="E6">
+        <v>5</v>
+      </c>
+      <c r="F6">
+        <v>5</v>
+      </c>
+      <c r="G6" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6" s="1">
+        <v>36530</v>
+      </c>
+      <c r="I6" s="1">
+        <v>36530</v>
+      </c>
+      <c r="J6" t="s">
+        <v>10</v>
+      </c>
+      <c r="K6" t="s">
+        <v>10</v>
+      </c>
+      <c r="L6">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>